<commit_message>
Assertion fixes Moved page level assertions to test level
</commit_message>
<xml_diff>
--- a/src/main/java/com/swaglab/data/login/LoginTestData.xlsx
+++ b/src/main/java/com/swaglab/data/login/LoginTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>LOGIN06</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>LOGIN07</t>
+  </si>
+  <si>
+    <t>visual_user</t>
   </si>
 </sst>
 </file>
@@ -405,7 +417,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -476,6 +488,24 @@
       </c>
       <c r="C6" s="1"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>